<commit_message>
chore(maintenance_alert): update version and enhance item info formatting
- Bump version from 1.1.5 to 1.2.0 and update release date
- Change default emoji from clipboard to gear for item info display
- Revamp HTML layout to a table format for clearer presentation
- Conditionally include "Работы" field only if it has data
- Style table cells for better readability and visual consistency
</commit_message>
<xml_diff>
--- a/Обслуживание ПК и шкафов АСУТП.xlsx
+++ b/Обслуживание ПК и шкафов АСУТП.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="423">
   <si>
     <t xml:space="preserve">ПК АСУ ТП</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">Место расположения</t>
   </si>
   <si>
-    <t xml:space="preserve">Выполнить</t>
+    <t xml:space="preserve">Работы</t>
   </si>
   <si>
     <t xml:space="preserve">Интервал ТО (дней)</t>
@@ -745,12 +745,18 @@
     <t xml:space="preserve">ПСУ-9</t>
   </si>
   <si>
+    <t xml:space="preserve">Серверный шкаф</t>
+  </si>
+  <si>
     <t xml:space="preserve">842CSC01A01</t>
   </si>
   <si>
     <t xml:space="preserve">Серверная АСУТП измельчение</t>
   </si>
   <si>
+    <t xml:space="preserve">Замена фильтров</t>
+  </si>
+  <si>
     <t xml:space="preserve">842CSC01A02</t>
   </si>
   <si>
@@ -1274,9 +1280,6 @@
   </si>
   <si>
     <t xml:space="preserve">Шкаф БУУ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Снять бакап</t>
   </si>
   <si>
     <t xml:space="preserve">Промплощадка. НХПВ</t>
@@ -2064,9 +2067,9 @@
   <dimension ref="A1:O48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="F43" activeCellId="0" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2113,7 +2116,7 @@
       </c>
       <c r="D2" s="7" t="n">
         <f aca="false">COUNTIF(K:K,"ОБСЛУЖИТЬ")</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E2" s="8" t="n">
         <f aca="false">COUNTIF(K:K,"Внимание")</f>
@@ -2121,11 +2124,11 @@
       </c>
       <c r="F2" s="9" t="n">
         <f aca="false">COUNTIF(K:K,"Не требуется")</f>
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="G2" s="10" t="str">
         <f aca="false">IF(C2&gt;0,ROUND(D2/ C2 * 100,1)&amp;"%","0%")</f>
-        <v>13,6%</v>
+        <v>6,8%</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
@@ -3111,15 +3114,15 @@
         <v>3</v>
       </c>
       <c r="I31" s="2" t="n">
-        <v>45843</v>
+        <v>45894</v>
       </c>
       <c r="J31" s="2" t="n">
         <f aca="false">I31+G31</f>
-        <v>45874</v>
+        <v>45925</v>
       </c>
       <c r="K31" s="16" t="str">
         <f aca="true">IF(J31&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J31-TODAY()&lt;=H31,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3139,6 +3142,9 @@
       <c r="E32" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="F32" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G32" s="1" t="n">
         <v>31</v>
       </c>
@@ -3146,15 +3152,15 @@
         <v>3</v>
       </c>
       <c r="I32" s="2" t="n">
-        <v>45843</v>
+        <v>45894</v>
       </c>
       <c r="J32" s="2" t="n">
         <f aca="false">I32+G32</f>
-        <v>45874</v>
+        <v>45925</v>
       </c>
       <c r="K32" s="16" t="str">
         <f aca="true">IF(J32&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J32-TODAY()&lt;=H32,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,6 +3180,9 @@
       <c r="E33" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="F33" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G33" s="1" t="n">
         <v>31</v>
       </c>
@@ -3181,15 +3190,15 @@
         <v>3</v>
       </c>
       <c r="I33" s="2" t="n">
-        <v>45843</v>
+        <v>45894</v>
       </c>
       <c r="J33" s="2" t="n">
         <f aca="false">I33+G33</f>
-        <v>45874</v>
+        <v>45925</v>
       </c>
       <c r="K33" s="16" t="str">
         <f aca="true">IF(J33&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J33-TODAY()&lt;=H33,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3454,6 +3463,9 @@
       <c r="E41" s="1" t="s">
         <v>83</v>
       </c>
+      <c r="F41" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G41" s="1" t="n">
         <v>31</v>
       </c>
@@ -3524,6 +3536,9 @@
       <c r="E43" s="1" t="s">
         <v>87</v>
       </c>
+      <c r="F43" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G43" s="1" t="n">
         <v>31</v>
       </c>
@@ -3558,6 +3573,9 @@
       </c>
       <c r="E44" s="1" t="s">
         <v>83</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>31</v>
@@ -3753,9 +3771,9 @@
   <dimension ref="A1:K272"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A233" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E264" activeCellId="0" sqref="E264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3805,7 +3823,7 @@
       </c>
       <c r="D2" s="7" t="n">
         <f aca="false">COUNTIF(K:K,"ОБСЛУЖИТЬ")</f>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E2" s="8" t="n">
         <f aca="false">COUNTIF(K:K,"Внимание")</f>
@@ -3813,11 +3831,11 @@
       </c>
       <c r="F2" s="9" t="n">
         <f aca="false">COUNTIF(K:K,"Не требуется")</f>
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="G2" s="10" t="str">
         <f aca="false">IF(C2&gt;0,ROUND(D2/ C2 * 100,1)&amp;"%","0%")</f>
-        <v>6,3%</v>
+        <v>4,4%</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
@@ -3884,7 +3902,7 @@
         <v>24</v>
       </c>
       <c r="G5" s="1" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>1</v>
@@ -3894,7 +3912,7 @@
       </c>
       <c r="J5" s="2" t="n">
         <f aca="false">I5+G5</f>
-        <v>45898</v>
+        <v>45905</v>
       </c>
       <c r="K5" s="16" t="str">
         <f aca="true">IF(J5&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J5-TODAY()&lt;=H5,"Внимание","Не требуется"))</f>
@@ -3919,7 +3937,7 @@
         <v>24</v>
       </c>
       <c r="G6" s="1" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>1</v>
@@ -3929,7 +3947,7 @@
       </c>
       <c r="J6" s="2" t="n">
         <f aca="false">I6+G6</f>
-        <v>45898</v>
+        <v>45905</v>
       </c>
       <c r="K6" s="16" t="str">
         <f aca="true">IF(J6&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J6-TODAY()&lt;=H6,"Внимание","Не требуется"))</f>
@@ -6788,6 +6806,9 @@
       <c r="E88" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="F88" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G88" s="1" t="n">
         <v>180</v>
       </c>
@@ -6823,6 +6844,9 @@
       <c r="E89" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="F89" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G89" s="1" t="n">
         <v>180</v>
       </c>
@@ -6858,6 +6882,9 @@
       <c r="E90" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="F90" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G90" s="1" t="n">
         <v>60</v>
       </c>
@@ -6893,6 +6920,9 @@
       <c r="E91" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="F91" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G91" s="1" t="n">
         <v>60</v>
       </c>
@@ -6928,6 +6958,9 @@
       <c r="E92" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="F92" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G92" s="1" t="n">
         <v>60</v>
       </c>
@@ -6963,6 +6996,9 @@
       <c r="E93" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="F93" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G93" s="1" t="n">
         <v>60</v>
       </c>
@@ -7410,30 +7446,33 @@
         <v>56</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>96</v>
+        <v>239</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="G106" s="1" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H106" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I106" s="2" t="n">
-        <v>45885</v>
+        <v>45894</v>
       </c>
       <c r="J106" s="2" t="n">
         <f aca="false">I106+G106</f>
-        <v>45892</v>
+        <v>45908</v>
       </c>
       <c r="K106" s="16" t="str">
         <f aca="true">IF(J106&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J106-TODAY()&lt;=H106,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7445,30 +7484,33 @@
         <v>56</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>96</v>
+        <v>239</v>
       </c>
       <c r="D107" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E107" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E107" s="1" t="s">
-        <v>240</v>
+      <c r="F107" s="1" t="s">
+        <v>242</v>
       </c>
       <c r="G107" s="1" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="H107" s="1" t="n">
         <v>1</v>
       </c>
       <c r="I107" s="2" t="n">
-        <v>45885</v>
+        <v>45894</v>
       </c>
       <c r="J107" s="2" t="n">
         <f aca="false">I107+G107</f>
-        <v>45892</v>
+        <v>45908</v>
       </c>
       <c r="K107" s="16" t="str">
         <f aca="true">IF(J107&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J107-TODAY()&lt;=H107,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7483,10 +7525,10 @@
         <v>99</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G108" s="1" t="n">
         <v>31</v>
@@ -7518,10 +7560,10 @@
         <v>102</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G109" s="1" t="n">
         <v>31</v>
@@ -7553,10 +7595,10 @@
         <v>102</v>
       </c>
       <c r="D110" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E110" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E110" s="1" t="s">
-        <v>243</v>
       </c>
       <c r="G110" s="1" t="n">
         <v>31</v>
@@ -7588,10 +7630,10 @@
         <v>102</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G111" s="1" t="n">
         <v>31</v>
@@ -7623,10 +7665,10 @@
         <v>102</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G112" s="1" t="n">
         <v>31</v>
@@ -7658,10 +7700,10 @@
         <v>102</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G113" s="1" t="n">
         <v>31</v>
@@ -7693,10 +7735,10 @@
         <v>99</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G114" s="1" t="n">
         <v>31</v>
@@ -7728,10 +7770,10 @@
         <v>102</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G115" s="1" t="n">
         <v>31</v>
@@ -7763,10 +7805,10 @@
         <v>102</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G116" s="1" t="n">
         <v>31</v>
@@ -7798,10 +7840,10 @@
         <v>99</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G117" s="1" t="n">
         <v>31</v>
@@ -7833,10 +7875,10 @@
         <v>102</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G118" s="1" t="n">
         <v>31</v>
@@ -7868,10 +7910,10 @@
         <v>102</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G119" s="1" t="n">
         <v>31</v>
@@ -7903,10 +7945,13 @@
         <v>102</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>121</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="G120" s="1" t="n">
         <v>31</v>
@@ -7938,10 +7983,10 @@
         <v>99</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G121" s="1" t="n">
         <v>31</v>
@@ -7973,10 +8018,10 @@
         <v>102</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G122" s="1" t="n">
         <v>31</v>
@@ -8008,7 +8053,7 @@
         <v>99</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>81</v>
@@ -8043,10 +8088,10 @@
         <v>99</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="G124" s="1" t="n">
         <v>31</v>
@@ -8078,10 +8123,10 @@
         <v>99</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G125" s="1" t="n">
         <v>31</v>
@@ -8113,10 +8158,10 @@
         <v>99</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G126" s="1" t="n">
         <v>31</v>
@@ -8148,10 +8193,10 @@
         <v>99</v>
       </c>
       <c r="D127" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>265</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>263</v>
       </c>
       <c r="G127" s="1" t="n">
         <v>31</v>
@@ -8183,10 +8228,10 @@
         <v>99</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="G128" s="1" t="n">
         <v>31</v>
@@ -8218,11 +8263,14 @@
         <v>99</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="F129" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G129" s="1" t="n">
         <v>31</v>
       </c>
@@ -8230,15 +8278,15 @@
         <v>3</v>
       </c>
       <c r="I129" s="2" t="n">
-        <v>45843</v>
+        <v>45894</v>
       </c>
       <c r="J129" s="2" t="n">
         <f aca="false">I129+G129</f>
-        <v>45874</v>
+        <v>45925</v>
       </c>
       <c r="K129" s="16" t="str">
         <f aca="true">IF(J129&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J129-TODAY()&lt;=H129,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8253,11 +8301,14 @@
         <v>99</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="F130" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G130" s="1" t="n">
         <v>31</v>
       </c>
@@ -8265,15 +8316,15 @@
         <v>3</v>
       </c>
       <c r="I130" s="2" t="n">
-        <v>45843</v>
+        <v>45894</v>
       </c>
       <c r="J130" s="2" t="n">
         <f aca="false">I130+G130</f>
-        <v>45874</v>
+        <v>45925</v>
       </c>
       <c r="K130" s="16" t="str">
         <f aca="true">IF(J130&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J130-TODAY()&lt;=H130,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8288,11 +8339,14 @@
         <v>99</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="E131" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="F131" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="G131" s="1" t="n">
         <v>31</v>
       </c>
@@ -8300,15 +8354,15 @@
         <v>3</v>
       </c>
       <c r="I131" s="2" t="n">
-        <v>45843</v>
+        <v>45894</v>
       </c>
       <c r="J131" s="2" t="n">
         <f aca="false">I131+G131</f>
-        <v>45874</v>
+        <v>45925</v>
       </c>
       <c r="K131" s="16" t="str">
         <f aca="true">IF(J131&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J131-TODAY()&lt;=H131,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8323,7 +8377,7 @@
         <v>99</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>173</v>
@@ -8358,10 +8412,10 @@
         <v>99</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="G133" s="1" t="n">
         <v>90</v>
@@ -8393,10 +8447,10 @@
         <v>99</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G134" s="1" t="n">
         <v>90</v>
@@ -8425,13 +8479,13 @@
         <v>56</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="G135" s="1" t="n">
         <v>90</v>
@@ -8501,7 +8555,7 @@
         <v>133</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G137" s="1" t="n">
         <v>31</v>
@@ -8536,7 +8590,7 @@
         <v>134</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="G138" s="1" t="n">
         <v>31</v>
@@ -8568,7 +8622,7 @@
         <v>221</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E139" s="1" t="s">
         <v>230</v>
@@ -8603,10 +8657,10 @@
         <v>221</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G140" s="1" t="n">
         <v>31</v>
@@ -8638,10 +8692,10 @@
         <v>221</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G141" s="1" t="n">
         <v>31</v>
@@ -8673,7 +8727,7 @@
         <v>221</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>238</v>
@@ -8708,7 +8762,7 @@
         <v>221</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E143" s="1" t="s">
         <v>238</v>
@@ -8743,10 +8797,10 @@
         <v>221</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G144" s="1" t="n">
         <v>31</v>
@@ -8778,7 +8832,7 @@
         <v>221</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="E145" s="1" t="s">
         <v>131</v>
@@ -8813,10 +8867,10 @@
         <v>221</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G146" s="1" t="n">
         <v>31</v>
@@ -8848,7 +8902,7 @@
         <v>221</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>224</v>
@@ -8883,10 +8937,10 @@
         <v>221</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E148" s="1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="G148" s="1" t="n">
         <v>31</v>
@@ -8918,10 +8972,10 @@
         <v>221</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="E149" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G149" s="1" t="n">
         <v>31</v>
@@ -8950,10 +9004,10 @@
         <v>56</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="E150" s="1" t="s">
         <v>131</v>
@@ -8985,13 +9039,13 @@
         <v>56</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G151" s="1" t="n">
         <v>31</v>
@@ -9020,13 +9074,13 @@
         <v>56</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G152" s="1" t="n">
         <v>31</v>
@@ -9055,13 +9109,13 @@
         <v>56</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G153" s="1" t="n">
         <v>31</v>
@@ -9090,10 +9144,10 @@
         <v>56</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E154" s="1" t="s">
         <v>230</v>
@@ -9125,13 +9179,13 @@
         <v>56</v>
       </c>
       <c r="C155" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D155" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E155" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="G155" s="1" t="n">
         <v>31</v>
@@ -9160,13 +9214,13 @@
         <v>56</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="G156" s="1" t="n">
         <v>31</v>
@@ -9195,13 +9249,13 @@
         <v>56</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G157" s="1" t="n">
         <v>31</v>
@@ -9230,10 +9284,10 @@
         <v>56</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E158" s="1" t="s">
         <v>238</v>
@@ -9268,10 +9322,10 @@
         <v>99</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G159" s="1" t="n">
         <v>31</v>
@@ -9303,10 +9357,10 @@
         <v>136</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="E160" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G160" s="1" t="n">
         <v>31</v>
@@ -9338,10 +9392,10 @@
         <v>136</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E161" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G161" s="1" t="n">
         <v>31</v>
@@ -9373,10 +9427,10 @@
         <v>136</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G162" s="1" t="n">
         <v>31</v>
@@ -9408,10 +9462,10 @@
         <v>136</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G163" s="1" t="n">
         <v>31</v>
@@ -9443,10 +9497,10 @@
         <v>136</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G164" s="1" t="n">
         <v>31</v>
@@ -9478,10 +9532,10 @@
         <v>136</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G165" s="1" t="n">
         <v>31</v>
@@ -9513,10 +9567,10 @@
         <v>136</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G166" s="1" t="n">
         <v>31</v>
@@ -9548,10 +9602,10 @@
         <v>136</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G167" s="1" t="n">
         <v>31</v>
@@ -9583,10 +9637,10 @@
         <v>166</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="G168" s="1" t="n">
         <v>31</v>
@@ -9618,10 +9672,10 @@
         <v>136</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G169" s="1" t="n">
         <v>31</v>
@@ -9653,10 +9707,10 @@
         <v>136</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G170" s="1" t="n">
         <v>31</v>
@@ -9688,10 +9742,10 @@
         <v>136</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="E171" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G171" s="1" t="n">
         <v>31</v>
@@ -9723,10 +9777,10 @@
         <v>136</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G172" s="1" t="n">
         <v>31</v>
@@ -9758,10 +9812,10 @@
         <v>136</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E173" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G173" s="1" t="n">
         <v>31</v>
@@ -9793,10 +9847,10 @@
         <v>136</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G174" s="1" t="n">
         <v>31</v>
@@ -9828,10 +9882,10 @@
         <v>136</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G175" s="1" t="n">
         <v>31</v>
@@ -9863,10 +9917,10 @@
         <v>136</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E176" s="1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="G176" s="1" t="n">
         <v>31</v>
@@ -9898,7 +9952,7 @@
         <v>166</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>123</v>
@@ -9933,7 +9987,7 @@
         <v>166</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>125</v>
@@ -9968,7 +10022,7 @@
         <v>99</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>125</v>
@@ -10003,7 +10057,7 @@
         <v>99</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>125</v>
@@ -10038,7 +10092,7 @@
         <v>99</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>125</v>
@@ -10073,7 +10127,7 @@
         <v>99</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>125</v>
@@ -10108,7 +10162,7 @@
         <v>99</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>125</v>
@@ -10143,10 +10197,10 @@
         <v>99</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E184" s="1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G184" s="1" t="n">
         <v>31</v>
@@ -10178,10 +10232,10 @@
         <v>99</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E185" s="1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G185" s="1" t="n">
         <v>31</v>
@@ -10213,7 +10267,7 @@
         <v>143</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>123</v>
@@ -10248,10 +10302,10 @@
         <v>99</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="E187" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="G187" s="1" t="n">
         <v>31</v>
@@ -10286,7 +10340,7 @@
         <v>203</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G188" s="1" t="n">
         <v>60</v>
@@ -10321,7 +10375,7 @@
         <v>205</v>
       </c>
       <c r="E189" s="1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G189" s="1" t="n">
         <v>60</v>
@@ -10353,7 +10407,7 @@
         <v>99</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>121</v>
@@ -10388,7 +10442,7 @@
         <v>99</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>121</v>
@@ -10423,7 +10477,7 @@
         <v>99</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>121</v>
@@ -10458,7 +10512,7 @@
         <v>99</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>121</v>
@@ -10493,7 +10547,7 @@
         <v>99</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>121</v>
@@ -10528,7 +10582,7 @@
         <v>99</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>121</v>
@@ -10563,7 +10617,7 @@
         <v>99</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>121</v>
@@ -10598,7 +10652,7 @@
         <v>99</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>121</v>
@@ -10633,7 +10687,7 @@
         <v>99</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>121</v>
@@ -10668,7 +10722,7 @@
         <v>99</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>121</v>
@@ -10703,7 +10757,7 @@
         <v>99</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E200" s="1" t="s">
         <v>121</v>
@@ -10738,7 +10792,7 @@
         <v>99</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="E201" s="1" t="s">
         <v>121</v>
@@ -10773,7 +10827,7 @@
         <v>99</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E202" s="1" t="s">
         <v>121</v>
@@ -10808,7 +10862,7 @@
         <v>99</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E203" s="1" t="s">
         <v>121</v>
@@ -10843,7 +10897,7 @@
         <v>99</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E204" s="1" t="s">
         <v>121</v>
@@ -10878,7 +10932,7 @@
         <v>99</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="E205" s="1" t="s">
         <v>121</v>
@@ -10913,10 +10967,10 @@
         <v>99</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G206" s="1" t="n">
         <v>31</v>
@@ -10948,10 +11002,10 @@
         <v>136</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="G207" s="1" t="n">
         <v>31</v>
@@ -10983,10 +11037,10 @@
         <v>99</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G208" s="1" t="n">
         <v>31</v>
@@ -11018,10 +11072,10 @@
         <v>136</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E209" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G209" s="1" t="n">
         <v>31</v>
@@ -11053,10 +11107,10 @@
         <v>99</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E210" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G210" s="1" t="n">
         <v>31</v>
@@ -11088,10 +11142,10 @@
         <v>136</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E211" s="1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="G211" s="1" t="n">
         <v>31</v>
@@ -11123,7 +11177,7 @@
         <v>99</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E212" s="1" t="s">
         <v>138</v>
@@ -11158,7 +11212,7 @@
         <v>99</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="E213" s="1" t="s">
         <v>138</v>
@@ -11193,7 +11247,7 @@
         <v>99</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E214" s="1" t="s">
         <v>138</v>
@@ -11228,7 +11282,7 @@
         <v>99</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="E215" s="1" t="s">
         <v>138</v>
@@ -11263,7 +11317,7 @@
         <v>99</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E216" s="1" t="s">
         <v>138</v>
@@ -11298,10 +11352,10 @@
         <v>99</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="E217" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G217" s="1" t="n">
         <v>31</v>
@@ -11333,10 +11387,10 @@
         <v>99</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E218" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G218" s="1" t="n">
         <v>31</v>
@@ -11368,10 +11422,10 @@
         <v>99</v>
       </c>
       <c r="D219" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="E219" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="E219" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="G219" s="1" t="n">
         <v>31</v>
@@ -11403,10 +11457,10 @@
         <v>99</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E220" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G220" s="1" t="n">
         <v>31</v>
@@ -11438,10 +11492,10 @@
         <v>99</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E221" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G221" s="1" t="n">
         <v>31</v>
@@ -11473,10 +11527,10 @@
         <v>99</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="E222" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G222" s="1" t="n">
         <v>31</v>
@@ -11508,10 +11562,10 @@
         <v>99</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E223" s="1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="G223" s="1" t="n">
         <v>31</v>
@@ -11543,10 +11597,10 @@
         <v>143</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E224" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G224" s="1" t="n">
         <v>31</v>
@@ -11578,10 +11632,10 @@
         <v>143</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E225" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G225" s="1" t="n">
         <v>31</v>
@@ -11613,10 +11667,10 @@
         <v>143</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="E226" s="1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G226" s="1" t="n">
         <v>31</v>
@@ -11648,10 +11702,10 @@
         <v>136</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E227" s="1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G227" s="1" t="n">
         <v>31</v>
@@ -11683,10 +11737,10 @@
         <v>136</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E228" s="1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G228" s="1" t="n">
         <v>31</v>
@@ -11718,10 +11772,10 @@
         <v>136</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E229" s="1" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G229" s="1" t="n">
         <v>31</v>
@@ -11753,10 +11807,10 @@
         <v>136</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="E230" s="1" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="G230" s="1" t="n">
         <v>31</v>
@@ -11788,10 +11842,10 @@
         <v>136</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E231" s="1" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="G231" s="1" t="n">
         <v>31</v>
@@ -11823,10 +11877,10 @@
         <v>136</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E232" s="1" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="G232" s="1" t="n">
         <v>31</v>
@@ -11858,10 +11912,10 @@
         <v>136</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E233" s="1" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="G233" s="1" t="n">
         <v>31</v>
@@ -11893,10 +11947,10 @@
         <v>136</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E234" s="1" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="G234" s="1" t="n">
         <v>31</v>
@@ -11928,10 +11982,10 @@
         <v>136</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E235" s="1" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="G235" s="1" t="n">
         <v>31</v>
@@ -11963,7 +12017,7 @@
         <v>99</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="E236" s="1" t="s">
         <v>91</v>
@@ -11998,7 +12052,7 @@
         <v>99</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E237" s="1" t="s">
         <v>91</v>
@@ -12033,7 +12087,7 @@
         <v>99</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E238" s="1" t="s">
         <v>91</v>
@@ -12068,7 +12122,7 @@
         <v>99</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E239" s="1" t="s">
         <v>91</v>
@@ -12103,7 +12157,7 @@
         <v>99</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="E240" s="1" t="s">
         <v>91</v>
@@ -12138,7 +12192,7 @@
         <v>99</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E241" s="1" t="s">
         <v>91</v>
@@ -12173,7 +12227,7 @@
         <v>99</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E242" s="1" t="s">
         <v>91</v>
@@ -12208,7 +12262,7 @@
         <v>99</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E243" s="1" t="s">
         <v>91</v>
@@ -12243,7 +12297,7 @@
         <v>99</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E244" s="1" t="s">
         <v>91</v>
@@ -12278,7 +12332,7 @@
         <v>99</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E245" s="1" t="s">
         <v>91</v>
@@ -12313,7 +12367,7 @@
         <v>99</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E246" s="1" t="s">
         <v>91</v>
@@ -12348,7 +12402,7 @@
         <v>99</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E247" s="1" t="s">
         <v>91</v>
@@ -12383,7 +12437,7 @@
         <v>99</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E248" s="1" t="s">
         <v>91</v>
@@ -12412,16 +12466,16 @@
         <v>245</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E249" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G249" s="1" t="n">
         <v>60</v>
@@ -12447,16 +12501,16 @@
         <v>246</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D250" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="E250" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="E250" s="1" t="s">
-        <v>404</v>
       </c>
       <c r="G250" s="1" t="n">
         <v>60</v>
@@ -12482,16 +12536,16 @@
         <v>247</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C251" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E251" s="1" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="G251" s="1" t="n">
         <v>60</v>
@@ -12517,16 +12571,16 @@
         <v>248</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C252" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E252" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="G252" s="1" t="n">
         <v>60</v>
@@ -12552,16 +12606,16 @@
         <v>249</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C253" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E253" s="1" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="G253" s="1" t="n">
         <v>60</v>
@@ -12587,16 +12641,16 @@
         <v>250</v>
       </c>
       <c r="B254" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C254" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="E254" s="1" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="G254" s="1" t="n">
         <v>60</v>
@@ -12622,19 +12676,19 @@
         <v>251</v>
       </c>
       <c r="B255" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C255" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="F255" s="1" t="s">
-        <v>416</v>
+        <v>65</v>
       </c>
       <c r="G255" s="1" t="n">
         <v>60</v>
@@ -12660,16 +12714,16 @@
         <v>252</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C256" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D256" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="E256" s="1" t="s">
         <v>418</v>
-      </c>
-      <c r="E256" s="1" t="s">
-        <v>417</v>
       </c>
       <c r="G256" s="1" t="n">
         <v>60</v>
@@ -12783,17 +12837,17 @@
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="18" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="18" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix(maintenance): rename column and update layout width for maintenance table
- Rename Excel column from "Выполнить" to "Работы"
- Update HTML table layout to increase width from 170px to 200px for multiple fields
- Correct conditional check and data formatting for the "Работы" field
- Adjust the styling to improve alignment and readability in maintenance info display
</commit_message>
<xml_diff>
--- a/Обслуживание ПК и шкафов АСУТП.xlsx
+++ b/Обслуживание ПК и шкафов АСУТП.xlsx
@@ -3773,7 +3773,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="4" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E264" activeCellId="0" sqref="E264"/>
+      <selection pane="bottomLeft" activeCell="I255" activeCellId="0" sqref="I255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12697,11 +12697,11 @@
         <v>3</v>
       </c>
       <c r="I255" s="2" t="n">
-        <v>45782</v>
+        <v>45833</v>
       </c>
       <c r="J255" s="2" t="n">
         <f aca="false">I255+G255</f>
-        <v>45842</v>
+        <v>45893</v>
       </c>
       <c r="K255" s="16" t="str">
         <f aca="true">IF(J255&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J255-TODAY()&lt;=H255,"Внимание","Не требуется"))</f>

</xml_diff>

<commit_message>
feat(excel): generate maintenance_data.xlsx file and attach in email
- Added function to create maintenance_data.xlsx from template with urgent maintenance data
- Populated Excel sheets with relevant data and current date in cell D1
- Improved error handling and logging during file generation
- Modified email sender to attach maintenance_data.xlsx file if provided
- Updated main app flow to generate and attach the maintenance data file when urgent items exist
- Removed all test scripts to clean up codebase and avoid redundant tests
</commit_message>
<xml_diff>
--- a/Обслуживание ПК и шкафов АСУТП.xlsx
+++ b/Обслуживание ПК и шкафов АСУТП.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17265" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ПК АСУ ТП" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
     <sheet name="вспомогательный" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_FD1" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$K$63</definedName>
+    <definedName name="_FD2" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$L$270</definedName>
+    <definedName name="_FD3" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$L$270</definedName>
     <definedName name="_FilterDatabase" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$K$63</definedName>
     <definedName name="_FilterDatabase" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$L$270</definedName>
   </definedNames>
@@ -2200,12 +2203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:O63"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2314,7 +2316,7 @@
       <c r="N4" s="14"/>
       <c r="O4" s="14"/>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -2351,7 +2353,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A48" si="2">A5+1</f>
         <v>2</v>
@@ -2389,7 +2391,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -2427,7 +2429,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -2465,7 +2467,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -2503,7 +2505,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -2541,7 +2543,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -2579,7 +2581,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -2617,7 +2619,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -2655,7 +2657,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -2693,7 +2695,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -2731,7 +2733,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -2769,7 +2771,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -2807,7 +2809,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -2845,7 +2847,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -2883,7 +2885,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -2921,7 +2923,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -2959,7 +2961,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -2997,7 +2999,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -3035,7 +3037,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -3073,7 +3075,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -3111,7 +3113,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -3149,7 +3151,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -3187,7 +3189,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -3225,7 +3227,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -3263,7 +3265,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -3301,7 +3303,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -3339,7 +3341,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -3377,7 +3379,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -3415,7 +3417,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -3453,7 +3455,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -3491,7 +3493,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -3529,7 +3531,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -3567,7 +3569,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -3605,7 +3607,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -3643,7 +3645,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -3681,7 +3683,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -3719,7 +3721,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -3795,7 +3797,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -3833,7 +3835,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -3871,7 +3873,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -3909,7 +3911,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -3947,7 +3949,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -3985,29 +3987,8 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="49" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A4:K63">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="ОБСЛУЖИТЬ"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:K63"/>
   <conditionalFormatting sqref="K5:K48">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"ОБСЛУЖИТЬ"</formula>
@@ -4026,13 +4007,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:L270"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C135" sqref="C135"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4080,11 +4060,11 @@
       </c>
       <c r="D2" s="7">
         <f ca="1">COUNTIF(K:K,"ОБСЛУЖИТЬ")</f>
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="E2" s="8">
         <f ca="1">COUNTIF(K:K,"Внимание")</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F2" s="9">
         <f ca="1">COUNTIF(K:K,"Не требуется")</f>
@@ -4140,7 +4120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
@@ -4177,7 +4157,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A69" si="2">A5+1</f>
         <v>2</v>
@@ -4215,7 +4195,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
@@ -4253,7 +4233,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -4291,7 +4271,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -4329,7 +4309,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -4367,7 +4347,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -4405,7 +4385,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -4443,7 +4423,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -4481,7 +4461,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -4519,7 +4499,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -4557,7 +4537,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -4595,7 +4575,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -4633,7 +4613,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -4671,7 +4651,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -4709,7 +4689,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -4747,7 +4727,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -4785,7 +4765,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -4823,7 +4803,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -4861,7 +4841,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -4899,7 +4879,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -4937,7 +4917,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -4975,7 +4955,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -5013,7 +4993,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -5051,7 +5031,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -5089,7 +5069,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -5127,7 +5107,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -5165,7 +5145,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -5203,7 +5183,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -5241,7 +5221,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -5279,7 +5259,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -5317,7 +5297,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -5355,7 +5335,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -5393,7 +5373,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -5431,7 +5411,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -5469,7 +5449,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -5507,7 +5487,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -5545,7 +5525,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -5583,7 +5563,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -5621,7 +5601,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -5659,7 +5639,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -5697,7 +5677,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -5735,7 +5715,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -5773,7 +5753,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -5811,7 +5791,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -5849,7 +5829,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -5887,7 +5867,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -5925,7 +5905,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="2"/>
         <v>48</v>
@@ -5963,7 +5943,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="2"/>
         <v>49</v>
@@ -6001,7 +5981,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -6039,7 +6019,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="2"/>
         <v>51</v>
@@ -6077,7 +6057,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="2"/>
         <v>52</v>
@@ -6115,7 +6095,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="2"/>
         <v>53</v>
@@ -6153,7 +6133,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="2"/>
         <v>54</v>
@@ -6191,7 +6171,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="2"/>
         <v>55</v>
@@ -6229,7 +6209,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="2"/>
         <v>56</v>
@@ -6267,7 +6247,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="2"/>
         <v>57</v>
@@ -6305,7 +6285,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="2"/>
         <v>58</v>
@@ -6343,7 +6323,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="2"/>
         <v>59</v>
@@ -6381,7 +6361,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -6419,7 +6399,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="2"/>
         <v>61</v>
@@ -6457,7 +6437,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="2"/>
         <v>62</v>
@@ -6495,7 +6475,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="2"/>
         <v>63</v>
@@ -6533,7 +6513,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="2"/>
         <v>64</v>
@@ -6571,7 +6551,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="2"/>
         <v>65</v>
@@ -6609,7 +6589,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" ref="A70:A133" si="5">A69+1</f>
         <v>66</v>
@@ -6647,7 +6627,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="5"/>
         <v>67</v>
@@ -6685,7 +6665,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="5"/>
         <v>68</v>
@@ -6723,7 +6703,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="5"/>
         <v>69</v>
@@ -6761,7 +6741,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="5"/>
         <v>70</v>
@@ -6799,7 +6779,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="5"/>
         <v>71</v>
@@ -6837,7 +6817,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="5"/>
         <v>72</v>
@@ -6875,7 +6855,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="5"/>
         <v>73</v>
@@ -6913,7 +6893,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="5"/>
         <v>74</v>
@@ -6951,7 +6931,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="5"/>
         <v>75</v>
@@ -6989,7 +6969,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="5"/>
         <v>76</v>
@@ -7027,7 +7007,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="5"/>
         <v>77</v>
@@ -7065,7 +7045,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="5"/>
         <v>78</v>
@@ -7103,7 +7083,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="5"/>
         <v>79</v>
@@ -7141,7 +7121,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="5"/>
         <v>80</v>
@@ -7179,7 +7159,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="5"/>
         <v>81</v>
@@ -7217,7 +7197,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="5"/>
         <v>82</v>
@@ -7255,7 +7235,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="5"/>
         <v>83</v>
@@ -7293,7 +7273,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="5"/>
         <v>84</v>
@@ -7331,7 +7311,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="5"/>
         <v>85</v>
@@ -7369,7 +7349,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="5"/>
         <v>86</v>
@@ -7407,7 +7387,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="5"/>
         <v>87</v>
@@ -7445,7 +7425,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="5"/>
         <v>88</v>
@@ -7483,7 +7463,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="5"/>
         <v>89</v>
@@ -7521,7 +7501,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="5"/>
         <v>90</v>
@@ -7559,7 +7539,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="5"/>
         <v>91</v>
@@ -7597,7 +7577,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <f t="shared" si="5"/>
         <v>92</v>
@@ -7635,7 +7615,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <f t="shared" si="5"/>
         <v>93</v>
@@ -7673,7 +7653,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <f t="shared" si="5"/>
         <v>94</v>
@@ -7711,7 +7691,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <f t="shared" si="5"/>
         <v>95</v>
@@ -7749,7 +7729,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <f t="shared" si="5"/>
         <v>96</v>
@@ -7787,7 +7767,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <f t="shared" si="5"/>
         <v>97</v>
@@ -7825,7 +7805,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <f t="shared" si="5"/>
         <v>98</v>
@@ -7863,7 +7843,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <f t="shared" si="5"/>
         <v>99</v>
@@ -7901,7 +7881,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <f t="shared" si="5"/>
         <v>100</v>
@@ -7939,7 +7919,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <f t="shared" si="5"/>
         <v>101</v>
@@ -7977,7 +7957,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <f t="shared" si="5"/>
         <v>102</v>
@@ -8012,10 +7992,10 @@
       </c>
       <c r="K106" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <f t="shared" si="5"/>
         <v>103</v>
@@ -8050,10 +8030,10 @@
       </c>
       <c r="K107" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="108" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <f t="shared" si="5"/>
         <v>104</v>
@@ -8088,10 +8068,10 @@
       </c>
       <c r="K108" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <f t="shared" si="5"/>
         <v>105</v>
@@ -8126,10 +8106,10 @@
       </c>
       <c r="K109" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <f t="shared" si="5"/>
         <v>106</v>
@@ -8164,10 +8144,10 @@
       </c>
       <c r="K110" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="111" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <f t="shared" si="5"/>
         <v>107</v>
@@ -8205,7 +8185,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="112" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <f t="shared" si="5"/>
         <v>108</v>
@@ -8240,10 +8220,10 @@
       </c>
       <c r="K112" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <f t="shared" si="5"/>
         <v>109</v>
@@ -8278,10 +8258,10 @@
       </c>
       <c r="K113" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <f t="shared" si="5"/>
         <v>110</v>
@@ -8316,10 +8296,10 @@
       </c>
       <c r="K114" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <f t="shared" si="5"/>
         <v>111</v>
@@ -8354,10 +8334,10 @@
       </c>
       <c r="K115" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <f t="shared" si="5"/>
         <v>112</v>
@@ -8392,10 +8372,10 @@
       </c>
       <c r="K116" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <f t="shared" si="5"/>
         <v>113</v>
@@ -8430,7 +8410,7 @@
       </c>
       <c r="K117" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
@@ -8471,7 +8451,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <f t="shared" si="5"/>
         <v>115</v>
@@ -8506,10 +8486,10 @@
       </c>
       <c r="K119" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <f t="shared" si="5"/>
         <v>116</v>
@@ -8544,10 +8524,10 @@
       </c>
       <c r="K120" s="16" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <f t="shared" si="5"/>
         <v>117</v>
@@ -8585,7 +8565,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <f t="shared" si="5"/>
         <v>118</v>
@@ -8623,7 +8603,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <f t="shared" si="5"/>
         <v>119</v>
@@ -8661,7 +8641,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <f t="shared" si="5"/>
         <v>120</v>
@@ -8699,7 +8679,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <f t="shared" si="5"/>
         <v>121</v>
@@ -8737,7 +8717,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <f t="shared" si="5"/>
         <v>122</v>
@@ -8775,7 +8755,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <f t="shared" si="5"/>
         <v>123</v>
@@ -8813,7 +8793,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <f t="shared" si="5"/>
         <v>124</v>
@@ -8851,7 +8831,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <f t="shared" si="5"/>
         <v>125</v>
@@ -8889,7 +8869,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <f t="shared" si="5"/>
         <v>126</v>
@@ -8927,7 +8907,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <f t="shared" si="5"/>
         <v>127</v>
@@ -8965,7 +8945,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <f t="shared" si="5"/>
         <v>128</v>
@@ -9003,7 +8983,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <f t="shared" si="5"/>
         <v>129</v>
@@ -9041,7 +9021,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <f t="shared" ref="A134:A197" si="8">A133+1</f>
         <v>130</v>
@@ -9076,7 +9056,7 @@
       </c>
       <c r="K134" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
@@ -9155,7 +9135,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <f t="shared" si="8"/>
         <v>133</v>
@@ -9190,10 +9170,10 @@
       </c>
       <c r="K137" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <f t="shared" si="8"/>
         <v>134</v>
@@ -9228,10 +9208,10 @@
       </c>
       <c r="K138" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <f t="shared" si="8"/>
         <v>135</v>
@@ -9266,10 +9246,10 @@
       </c>
       <c r="K139" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <f t="shared" si="8"/>
         <v>136</v>
@@ -9304,10 +9284,10 @@
       </c>
       <c r="K140" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <f t="shared" si="8"/>
         <v>137</v>
@@ -9342,10 +9322,10 @@
       </c>
       <c r="K141" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <f t="shared" si="8"/>
         <v>138</v>
@@ -9380,7 +9360,7 @@
       </c>
       <c r="K142" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
@@ -9421,7 +9401,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <f t="shared" si="8"/>
         <v>140</v>
@@ -9456,10 +9436,10 @@
       </c>
       <c r="K144" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <f t="shared" si="8"/>
         <v>141</v>
@@ -9494,10 +9474,10 @@
       </c>
       <c r="K145" s="16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <f t="shared" si="8"/>
         <v>142</v>
@@ -9535,7 +9515,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <f t="shared" si="8"/>
         <v>143</v>
@@ -9573,7 +9553,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <f t="shared" si="8"/>
         <v>144</v>
@@ -9611,7 +9591,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <f t="shared" si="8"/>
         <v>145</v>
@@ -9649,7 +9629,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <f t="shared" si="8"/>
         <v>146</v>
@@ -9687,7 +9667,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <f t="shared" si="8"/>
         <v>147</v>
@@ -9725,7 +9705,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <f t="shared" si="8"/>
         <v>148</v>
@@ -9763,7 +9743,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <f t="shared" si="8"/>
         <v>149</v>
@@ -9801,7 +9781,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <f t="shared" si="8"/>
         <v>150</v>
@@ -9839,7 +9819,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <f t="shared" si="8"/>
         <v>151</v>
@@ -9877,7 +9857,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <f t="shared" si="8"/>
         <v>152</v>
@@ -9915,7 +9895,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <f t="shared" si="8"/>
         <v>153</v>
@@ -9953,7 +9933,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <f t="shared" si="8"/>
         <v>154</v>
@@ -9991,7 +9971,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <f t="shared" si="8"/>
         <v>155</v>
@@ -10029,7 +10009,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <f t="shared" si="8"/>
         <v>156</v>
@@ -10067,7 +10047,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <f t="shared" si="8"/>
         <v>157</v>
@@ -10105,7 +10085,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <f t="shared" si="8"/>
         <v>158</v>
@@ -10143,7 +10123,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <f t="shared" si="8"/>
         <v>159</v>
@@ -10181,7 +10161,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <f t="shared" si="8"/>
         <v>160</v>
@@ -10219,7 +10199,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <f t="shared" si="8"/>
         <v>161</v>
@@ -10257,7 +10237,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <f t="shared" si="8"/>
         <v>162</v>
@@ -10295,7 +10275,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <f t="shared" si="8"/>
         <v>163</v>
@@ -10333,7 +10313,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <f t="shared" si="8"/>
         <v>164</v>
@@ -10371,7 +10351,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <f t="shared" si="8"/>
         <v>165</v>
@@ -10409,7 +10389,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <f t="shared" si="8"/>
         <v>166</v>
@@ -10447,7 +10427,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <f t="shared" si="8"/>
         <v>167</v>
@@ -10485,7 +10465,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <f t="shared" si="8"/>
         <v>168</v>
@@ -10523,7 +10503,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <f t="shared" si="8"/>
         <v>169</v>
@@ -10561,7 +10541,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <f t="shared" si="8"/>
         <v>170</v>
@@ -10599,7 +10579,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <f t="shared" si="8"/>
         <v>171</v>
@@ -10637,7 +10617,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <f t="shared" si="8"/>
         <v>172</v>
@@ -10865,7 +10845,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <f t="shared" si="8"/>
         <v>178</v>
@@ -10903,7 +10883,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <f t="shared" si="8"/>
         <v>179</v>
@@ -10941,7 +10921,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <f t="shared" si="8"/>
         <v>180</v>
@@ -10979,7 +10959,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <f t="shared" si="8"/>
         <v>181</v>
@@ -11017,7 +10997,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <f t="shared" si="8"/>
         <v>182</v>
@@ -11055,7 +11035,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <f t="shared" si="8"/>
         <v>183</v>
@@ -11093,7 +11073,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <f t="shared" si="8"/>
         <v>184</v>
@@ -11131,7 +11111,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <f t="shared" si="8"/>
         <v>185</v>
@@ -11169,7 +11149,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <f t="shared" si="8"/>
         <v>186</v>
@@ -11207,7 +11187,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <f t="shared" si="8"/>
         <v>187</v>
@@ -11245,7 +11225,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <f t="shared" si="8"/>
         <v>188</v>
@@ -11283,7 +11263,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <f t="shared" si="8"/>
         <v>189</v>
@@ -11321,7 +11301,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <f t="shared" si="8"/>
         <v>190</v>
@@ -11359,7 +11339,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <f t="shared" si="8"/>
         <v>191</v>
@@ -11397,7 +11377,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <f t="shared" si="8"/>
         <v>192</v>
@@ -11435,7 +11415,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <f t="shared" si="8"/>
         <v>193</v>
@@ -11473,7 +11453,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <f t="shared" ref="A198:A254" si="11">A197+1</f>
         <v>194</v>
@@ -11511,7 +11491,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <f t="shared" si="11"/>
         <v>195</v>
@@ -11549,7 +11529,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <f t="shared" si="11"/>
         <v>196</v>
@@ -11587,7 +11567,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <f t="shared" si="11"/>
         <v>197</v>
@@ -11625,7 +11605,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <f t="shared" si="11"/>
         <v>198</v>
@@ -11663,7 +11643,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <f t="shared" si="11"/>
         <v>199</v>
@@ -11701,7 +11681,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <f t="shared" si="11"/>
         <v>200</v>
@@ -11739,7 +11719,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <f t="shared" si="11"/>
         <v>201</v>
@@ -11777,7 +11757,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <f t="shared" si="11"/>
         <v>202</v>
@@ -11815,7 +11795,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <f t="shared" si="11"/>
         <v>203</v>
@@ -11853,7 +11833,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <f t="shared" si="11"/>
         <v>204</v>
@@ -11891,7 +11871,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <f t="shared" si="11"/>
         <v>205</v>
@@ -11929,7 +11909,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <f t="shared" si="11"/>
         <v>206</v>
@@ -11967,7 +11947,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <f t="shared" si="11"/>
         <v>207</v>
@@ -12005,7 +11985,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <f t="shared" si="11"/>
         <v>208</v>
@@ -12043,7 +12023,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <f t="shared" si="11"/>
         <v>209</v>
@@ -12081,7 +12061,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <f t="shared" si="11"/>
         <v>210</v>
@@ -12119,7 +12099,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <f t="shared" si="11"/>
         <v>211</v>
@@ -12157,7 +12137,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <f t="shared" si="11"/>
         <v>212</v>
@@ -12195,7 +12175,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <f t="shared" si="11"/>
         <v>213</v>
@@ -12233,7 +12213,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <f t="shared" si="11"/>
         <v>214</v>
@@ -12271,7 +12251,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <f t="shared" si="11"/>
         <v>215</v>
@@ -12309,7 +12289,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <f t="shared" si="11"/>
         <v>216</v>
@@ -12347,7 +12327,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <f t="shared" si="11"/>
         <v>217</v>
@@ -12385,7 +12365,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <f t="shared" si="11"/>
         <v>218</v>
@@ -12420,10 +12400,10 @@
       </c>
       <c r="K222" s="16" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <f t="shared" si="11"/>
         <v>219</v>
@@ -12458,10 +12438,10 @@
       </c>
       <c r="K223" s="16" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <f t="shared" si="11"/>
         <v>220</v>
@@ -12496,10 +12476,10 @@
       </c>
       <c r="K224" s="16" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>Внимание</v>
-      </c>
-    </row>
-    <row r="225" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>ОБСЛУЖИТЬ</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <f t="shared" si="11"/>
         <v>221</v>
@@ -12537,7 +12517,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="226" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <f t="shared" si="11"/>
         <v>222</v>
@@ -12575,7 +12555,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="227" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <f t="shared" si="11"/>
         <v>223</v>
@@ -12613,7 +12593,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="228" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <f t="shared" si="11"/>
         <v>224</v>
@@ -12651,7 +12631,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="229" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <f t="shared" si="11"/>
         <v>225</v>
@@ -12689,7 +12669,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="230" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <f t="shared" si="11"/>
         <v>226</v>
@@ -12727,7 +12707,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="231" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <f t="shared" si="11"/>
         <v>227</v>
@@ -12765,7 +12745,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="232" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <f t="shared" si="11"/>
         <v>228</v>
@@ -12803,7 +12783,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="233" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <f t="shared" si="11"/>
         <v>229</v>
@@ -12841,7 +12821,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="234" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <f t="shared" si="11"/>
         <v>230</v>
@@ -12879,7 +12859,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="235" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <f t="shared" si="11"/>
         <v>231</v>
@@ -12917,7 +12897,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="236" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <f t="shared" si="11"/>
         <v>232</v>
@@ -12955,7 +12935,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="237" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <f t="shared" si="11"/>
         <v>233</v>
@@ -12993,7 +12973,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="238" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <f t="shared" si="11"/>
         <v>234</v>
@@ -13031,7 +13011,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="239" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <f t="shared" si="11"/>
         <v>235</v>
@@ -13069,7 +13049,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="240" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <f t="shared" si="11"/>
         <v>236</v>
@@ -13107,7 +13087,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <f t="shared" si="11"/>
         <v>237</v>
@@ -13145,7 +13125,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <f t="shared" si="11"/>
         <v>238</v>
@@ -13183,7 +13163,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <f t="shared" si="11"/>
         <v>239</v>
@@ -13221,7 +13201,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <f t="shared" si="11"/>
         <v>240</v>
@@ -13259,7 +13239,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <f t="shared" si="11"/>
         <v>241</v>
@@ -13297,7 +13277,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <f t="shared" si="11"/>
         <v>242</v>
@@ -13335,7 +13315,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <f t="shared" si="11"/>
         <v>243</v>
@@ -13373,7 +13353,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <f t="shared" si="11"/>
         <v>244</v>
@@ -13411,7 +13391,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <f t="shared" si="11"/>
         <v>245</v>
@@ -13449,7 +13429,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <f t="shared" si="11"/>
         <v>246</v>
@@ -13487,7 +13467,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <f t="shared" si="11"/>
         <v>247</v>
@@ -13525,7 +13505,7 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <f t="shared" si="11"/>
         <v>248</v>
@@ -13601,7 +13581,7 @@
         <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
-    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <f t="shared" si="11"/>
         <v>250</v>
@@ -13639,63 +13619,56 @@
         <v>Не требуется</v>
       </c>
     </row>
-    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K255" s="16"/>
     </row>
-    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K256" s="16"/>
     </row>
-    <row r="257" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="257" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K257" s="16"/>
     </row>
-    <row r="258" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="258" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K258" s="16"/>
     </row>
-    <row r="259" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="259" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K259" s="16"/>
     </row>
-    <row r="260" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K260" s="16"/>
     </row>
-    <row r="261" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="261" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K261" s="16"/>
     </row>
-    <row r="262" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="262" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K262" s="16"/>
     </row>
-    <row r="263" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K263" s="16"/>
     </row>
-    <row r="264" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="264" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K264" s="16"/>
     </row>
-    <row r="265" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="265" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K265" s="16"/>
     </row>
-    <row r="266" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="266" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K266" s="16"/>
     </row>
-    <row r="267" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="267" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K267" s="16"/>
     </row>
-    <row r="268" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K268" s="16"/>
     </row>
-    <row r="269" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="269" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K269" s="16"/>
     </row>
-    <row r="270" spans="11:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="270" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K270" s="16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:L270">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="Внимание"/>
-        <filter val="ОБСЛУЖИТЬ"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A4:L270"/>
   <conditionalFormatting sqref="K5:K254">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"ОБСЛУЖИТЬ"</formula>

</xml_diff>

<commit_message>
feat(maintenance): add equipment mark-as-serviced feature with UI support
- Implement method to update last maintenance date in Excel for specified equipment
- Add POST endpoints for marking single and multiple equipment items as serviced
- Improve dashboard UI with success/error messages for servicing operations
- Add checkboxes and buttons for bulk marking equipment as serviced in urgent and warning lists
- Implement client-side JavaScript to handle bulk serviced submission with confirmation
- Ensure filter parameters are preserved during redirects after servicing actions
</commit_message>
<xml_diff>
--- a/Обслуживание ПК и шкафов АСУТП.xlsx
+++ b/Обслуживание ПК и шкафов АСУТП.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Обслуживание оборудования АСУТП\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\7Arrt\Desktop\Projects\maintenance_alert\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,8 +17,8 @@
     <sheet name="вспомогательный" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$K$47</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$K$279</definedName>
+    <definedName name="_FilterDatabase" localSheetId="0" hidden="1">'ПК АСУ ТП'!$A$4:$K$47</definedName>
+    <definedName name="_FilterDatabase" localSheetId="1" hidden="1">'Шкафы АСУ ТП'!$A$4:$K$279</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -2415,15 +2415,15 @@
       </c>
       <c r="D2" s="7">
         <f ca="1">COUNTIF(K:K,"ОБСЛУЖИТЬ")</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="8">
         <f ca="1">COUNTIF(K:K,"Внимание")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="9">
         <f ca="1">COUNTIF(K:K,"Не требуется")</f>
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -2577,15 +2577,15 @@
         <v>3</v>
       </c>
       <c r="I7" s="2">
-        <v>45983</v>
+        <v>46031.147372685184</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>46014</v>
+        <v>46062.147372685184</v>
       </c>
       <c r="K7" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2653,15 +2653,15 @@
         <v>3</v>
       </c>
       <c r="I9" s="2">
-        <v>45963</v>
+        <v>46031.151493055557</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>46025</v>
+        <v>46093.151493055557</v>
       </c>
       <c r="K9" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -3261,15 +3261,15 @@
         <v>3</v>
       </c>
       <c r="I25" s="2">
-        <v>45983</v>
+        <v>46031.14738425926</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>46014</v>
+        <v>46062.14738425926</v>
       </c>
       <c r="K25" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="K37" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -3793,15 +3793,15 @@
         <v>3</v>
       </c>
       <c r="I39" s="2">
-        <v>45995</v>
+        <v>46031.144618055558</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>46026</v>
+        <v>46062.144618055558</v>
       </c>
       <c r="K39" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -4209,15 +4209,15 @@
       </c>
       <c r="D2" s="7">
         <f ca="1">COUNTIF(K:K,"ОБСЛУЖИТЬ")</f>
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="E2" s="8">
         <f ca="1">COUNTIF(K:K,"Внимание")</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F2" s="9">
         <f ca="1">COUNTIF(K:K,"Не требуется")</f>
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5136,7 +5136,7 @@
       </c>
       <c r="K27" s="16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="K28" s="16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="K29" s="16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="K37" s="16" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>Внимание</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -13982,15 +13982,15 @@
         <v>3</v>
       </c>
       <c r="I260" s="15">
-        <v>45983</v>
+        <v>46031.147418981483</v>
       </c>
       <c r="J260" s="2">
         <f t="shared" si="10"/>
-        <v>46014</v>
+        <v>46062.147418981483</v>
       </c>
       <c r="K260" s="16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.25">
@@ -14020,15 +14020,15 @@
         <v>3</v>
       </c>
       <c r="I261" s="2">
-        <v>45995</v>
+        <v>46031.144537037035</v>
       </c>
       <c r="J261" s="2">
         <f t="shared" ref="J261:J279" si="14">I261+G261</f>
-        <v>46026</v>
+        <v>46062.144537037035</v>
       </c>
       <c r="K261" s="16" t="str">
         <f t="shared" ref="K261:K279" ca="1" si="15">IF(J261&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J261-TODAY()&lt;=H261,"Внимание","Не требуется"))</f>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
@@ -14058,15 +14058,15 @@
         <v>3</v>
       </c>
       <c r="I262" s="2">
-        <v>45963</v>
+        <v>46031.150625000002</v>
       </c>
       <c r="J262" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150625000002</v>
       </c>
       <c r="K262" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
@@ -14096,15 +14096,15 @@
         <v>3</v>
       </c>
       <c r="I263" s="2">
-        <v>45963</v>
+        <v>46031.150659722225</v>
       </c>
       <c r="J263" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150659722225</v>
       </c>
       <c r="K263" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
@@ -14134,15 +14134,15 @@
         <v>3</v>
       </c>
       <c r="I264" s="2">
-        <v>45963</v>
+        <v>46031.150682870371</v>
       </c>
       <c r="J264" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150682870371</v>
       </c>
       <c r="K264" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="265" spans="1:11" x14ac:dyDescent="0.25">
@@ -14172,15 +14172,15 @@
         <v>3</v>
       </c>
       <c r="I265" s="2">
-        <v>45963</v>
+        <v>46031.150717592594</v>
       </c>
       <c r="J265" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150717592594</v>
       </c>
       <c r="K265" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.25">
@@ -14210,15 +14210,15 @@
         <v>3</v>
       </c>
       <c r="I266" s="2">
-        <v>45963</v>
+        <v>46031.150740740741</v>
       </c>
       <c r="J266" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150740740741</v>
       </c>
       <c r="K266" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.25">
@@ -14248,15 +14248,15 @@
         <v>3</v>
       </c>
       <c r="I267" s="2">
-        <v>45963</v>
+        <v>46031.150775462964</v>
       </c>
       <c r="J267" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150775462964</v>
       </c>
       <c r="K267" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.25">
@@ -14286,15 +14286,15 @@
         <v>3</v>
       </c>
       <c r="I268" s="2">
-        <v>45963</v>
+        <v>46031.15079861111</v>
       </c>
       <c r="J268" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.15079861111</v>
       </c>
       <c r="K268" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.25">
@@ -14324,15 +14324,15 @@
         <v>3</v>
       </c>
       <c r="I269" s="2">
-        <v>45963</v>
+        <v>46031.150833333333</v>
       </c>
       <c r="J269" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150833333333</v>
       </c>
       <c r="K269" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
@@ -14362,15 +14362,15 @@
         <v>3</v>
       </c>
       <c r="I270" s="2">
-        <v>45963</v>
+        <v>46031.150856481479</v>
       </c>
       <c r="J270" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150856481479</v>
       </c>
       <c r="K270" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.25">
@@ -14400,15 +14400,15 @@
         <v>3</v>
       </c>
       <c r="I271" s="2">
-        <v>45963</v>
+        <v>46031.150891203702</v>
       </c>
       <c r="J271" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150891203702</v>
       </c>
       <c r="K271" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.25">
@@ -14438,15 +14438,15 @@
         <v>3</v>
       </c>
       <c r="I272" s="2">
-        <v>45963</v>
+        <v>46031.150914351849</v>
       </c>
       <c r="J272" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150914351849</v>
       </c>
       <c r="K272" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.25">
@@ -14476,15 +14476,15 @@
         <v>3</v>
       </c>
       <c r="I273" s="2">
-        <v>45963</v>
+        <v>46031.150949074072</v>
       </c>
       <c r="J273" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.150949074072</v>
       </c>
       <c r="K273" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.25">
@@ -14514,15 +14514,15 @@
         <v>3</v>
       </c>
       <c r="I274" s="2">
-        <v>45963</v>
+        <v>46031.149988425925</v>
       </c>
       <c r="J274" s="2">
         <f t="shared" si="14"/>
-        <v>46023</v>
+        <v>46091.149988425925</v>
       </c>
       <c r="K274" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -14628,15 +14628,15 @@
         <v>3</v>
       </c>
       <c r="I277" s="2">
-        <v>45922</v>
+        <v>46031.150011574071</v>
       </c>
       <c r="J277" s="2">
         <f t="shared" si="14"/>
-        <v>46012</v>
+        <v>46121.150011574071</v>
       </c>
       <c r="K277" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
feat(maintenance): add Excel file backup and locking checks
- Introduce backup directory for Excel files under backups_excel
- Implement file lock check to prevent editing when Excel file is open
- Add automatic backup creation before marking equipment as serviced
- Prevent bulk servicing if Excel file is locked by another program
- Update dashboard statistics on page load automatically
- Enhance urgent and warning checkbox styles with accent colors for better UX
</commit_message>
<xml_diff>
--- a/Обслуживание ПК и шкафов АСУТП.xlsx
+++ b/Обслуживание ПК и шкафов АСУТП.xlsx
@@ -2577,11 +2577,11 @@
         <v>3</v>
       </c>
       <c r="I7" s="2">
-        <v>46031.147372685184</v>
+        <v>46031.204236111109</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>46062.147372685184</v>
+        <v>46062.204236111109</v>
       </c>
       <c r="K7" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2653,15 +2653,15 @@
         <v>3</v>
       </c>
       <c r="I9" s="2">
-        <v>46031.151493055557</v>
+        <v>45963</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>46093.151493055557</v>
+        <v>46025</v>
       </c>
       <c r="K9" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Не требуется</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -3261,11 +3261,11 @@
         <v>3</v>
       </c>
       <c r="I25" s="2">
-        <v>46031.14738425926</v>
+        <v>46031.204247685186</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>46062.14738425926</v>
+        <v>46062.204247685186</v>
       </c>
       <c r="K25" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -3793,11 +3793,11 @@
         <v>3</v>
       </c>
       <c r="I39" s="2">
-        <v>46031.144618055558</v>
+        <v>46031.203888888886</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>46062.144618055558</v>
+        <v>46062.203888888886</v>
       </c>
       <c r="K39" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4059,15 +4059,15 @@
         <v>3</v>
       </c>
       <c r="I46" s="2">
-        <v>45970</v>
+        <v>46031.206516203703</v>
       </c>
       <c r="J46" s="2">
         <f t="shared" si="0"/>
-        <v>46001</v>
+        <v>46062.206516203703</v>
       </c>
       <c r="K46" s="16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>ОБСЛУЖИТЬ</v>
+        <v>Не требуется</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -4209,7 +4209,7 @@
       </c>
       <c r="D2" s="7">
         <f ca="1">COUNTIF(K:K,"ОБСЛУЖИТЬ")</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E2" s="8">
         <f ca="1">COUNTIF(K:K,"Внимание")</f>
@@ -4217,7 +4217,7 @@
       </c>
       <c r="F2" s="9">
         <f ca="1">COUNTIF(K:K,"Не требуется")</f>
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -13982,11 +13982,11 @@
         <v>3</v>
       </c>
       <c r="I260" s="15">
-        <v>46031.147418981483</v>
+        <v>46031.204270833332</v>
       </c>
       <c r="J260" s="2">
         <f t="shared" si="10"/>
-        <v>46062.147418981483</v>
+        <v>46062.204270833332</v>
       </c>
       <c r="K260" s="16" t="str">
         <f t="shared" ca="1" si="11"/>
@@ -14020,11 +14020,11 @@
         <v>3</v>
       </c>
       <c r="I261" s="2">
-        <v>46031.144537037035</v>
+        <v>46031.203912037039</v>
       </c>
       <c r="J261" s="2">
         <f t="shared" ref="J261:J279" si="14">I261+G261</f>
-        <v>46062.144537037035</v>
+        <v>46062.203912037039</v>
       </c>
       <c r="K261" s="16" t="str">
         <f t="shared" ref="K261:K279" ca="1" si="15">IF(J261&lt;=TODAY(),"ОБСЛУЖИТЬ",IF(J261-TODAY()&lt;=H261,"Внимание","Не требуется"))</f>
@@ -14058,11 +14058,11 @@
         <v>3</v>
       </c>
       <c r="I262" s="2">
-        <v>46031.150625000002</v>
+        <v>46031.20480324074</v>
       </c>
       <c r="J262" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150625000002</v>
+        <v>46091.20480324074</v>
       </c>
       <c r="K262" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14096,11 +14096,11 @@
         <v>3</v>
       </c>
       <c r="I263" s="2">
-        <v>46031.150659722225</v>
+        <v>46031.204826388886</v>
       </c>
       <c r="J263" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150659722225</v>
+        <v>46091.204826388886</v>
       </c>
       <c r="K263" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14134,11 +14134,11 @@
         <v>3</v>
       </c>
       <c r="I264" s="2">
-        <v>46031.150682870371</v>
+        <v>46031.204861111109</v>
       </c>
       <c r="J264" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150682870371</v>
+        <v>46091.204861111109</v>
       </c>
       <c r="K264" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14172,11 +14172,11 @@
         <v>3</v>
       </c>
       <c r="I265" s="2">
-        <v>46031.150717592594</v>
+        <v>46031.204884259256</v>
       </c>
       <c r="J265" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150717592594</v>
+        <v>46091.204884259256</v>
       </c>
       <c r="K265" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14210,11 +14210,11 @@
         <v>3</v>
       </c>
       <c r="I266" s="2">
-        <v>46031.150740740741</v>
+        <v>46031.204907407409</v>
       </c>
       <c r="J266" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150740740741</v>
+        <v>46091.204907407409</v>
       </c>
       <c r="K266" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14248,11 +14248,11 @@
         <v>3</v>
       </c>
       <c r="I267" s="2">
-        <v>46031.150775462964</v>
+        <v>46031.204942129632</v>
       </c>
       <c r="J267" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150775462964</v>
+        <v>46091.204942129632</v>
       </c>
       <c r="K267" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14286,11 +14286,11 @@
         <v>3</v>
       </c>
       <c r="I268" s="2">
-        <v>46031.15079861111</v>
+        <v>46031.204965277779</v>
       </c>
       <c r="J268" s="2">
         <f t="shared" si="14"/>
-        <v>46091.15079861111</v>
+        <v>46091.204965277779</v>
       </c>
       <c r="K268" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14324,11 +14324,11 @@
         <v>3</v>
       </c>
       <c r="I269" s="2">
-        <v>46031.150833333333</v>
+        <v>46031.205000000002</v>
       </c>
       <c r="J269" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150833333333</v>
+        <v>46091.205000000002</v>
       </c>
       <c r="K269" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14362,11 +14362,11 @@
         <v>3</v>
       </c>
       <c r="I270" s="2">
-        <v>46031.150856481479</v>
+        <v>46031.205034722225</v>
       </c>
       <c r="J270" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150856481479</v>
+        <v>46091.205034722225</v>
       </c>
       <c r="K270" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14400,11 +14400,11 @@
         <v>3</v>
       </c>
       <c r="I271" s="2">
-        <v>46031.150891203702</v>
+        <v>46031.205057870371</v>
       </c>
       <c r="J271" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150891203702</v>
+        <v>46091.205057870371</v>
       </c>
       <c r="K271" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14438,11 +14438,11 @@
         <v>3</v>
       </c>
       <c r="I272" s="2">
-        <v>46031.150914351849</v>
+        <v>46031.205092592594</v>
       </c>
       <c r="J272" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150914351849</v>
+        <v>46091.205092592594</v>
       </c>
       <c r="K272" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14476,11 +14476,11 @@
         <v>3</v>
       </c>
       <c r="I273" s="2">
-        <v>46031.150949074072</v>
+        <v>46031.20511574074</v>
       </c>
       <c r="J273" s="2">
         <f t="shared" si="14"/>
-        <v>46091.150949074072</v>
+        <v>46091.20511574074</v>
       </c>
       <c r="K273" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14514,11 +14514,11 @@
         <v>3</v>
       </c>
       <c r="I274" s="2">
-        <v>46031.149988425925</v>
+        <v>46031.205150462964</v>
       </c>
       <c r="J274" s="2">
         <f t="shared" si="14"/>
-        <v>46091.149988425925</v>
+        <v>46091.205150462964</v>
       </c>
       <c r="K274" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
@@ -14628,15 +14628,15 @@
         <v>3</v>
       </c>
       <c r="I277" s="2">
-        <v>46031.150011574071</v>
+        <v>45922</v>
       </c>
       <c r="J277" s="2">
         <f t="shared" si="14"/>
-        <v>46121.150011574071</v>
+        <v>46012</v>
       </c>
       <c r="K277" s="16" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>Не требуется</v>
+        <v>ОБСЛУЖИТЬ</v>
       </c>
     </row>
     <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
chore(config): update version to 2.0.0 for upcoming release
- Bump Config.VERSION from 1.5.0 to 2.0.0
- Add clickable refresh link with icon hover effect in dashboard header
- Implement loading animation replacing icon with GIF and fading effect
- Disable buttons and refresh link during loading to prevent multiple submits
- Attach event listeners to show loading animation on form submission and refresh link click
</commit_message>
<xml_diff>
--- a/Обслуживание ПК и шкафов АСУТП.xlsx
+++ b/Обслуживание ПК и шкафов АСУТП.xlsx
@@ -1122,7 +1122,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="22" t="n">
-        <v>46031.2647009375</v>
+        <v>46031.90153257479</v>
       </c>
       <c r="J7" s="22">
         <f>I7+G7</f>
@@ -1216,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="I9" s="22" t="n">
-        <v>46031.26437233797</v>
+        <v>45963</v>
       </c>
       <c r="J9" s="22">
         <f>I9+G9</f>
@@ -1968,7 +1968,7 @@
         <v>3</v>
       </c>
       <c r="I25" s="22" t="n">
-        <v>46031.26470232639</v>
+        <v>45983</v>
       </c>
       <c r="J25" s="22">
         <f>I25+G25</f>
@@ -2062,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="I27" s="22" t="n">
-        <v>46031.26339525463</v>
+        <v>45995</v>
       </c>
       <c r="J27" s="22">
         <f>I27+G27</f>
@@ -3002,7 +3002,7 @@
         <v>3</v>
       </c>
       <c r="I47" s="25" t="n">
-        <v>46031.26537509259</v>
+        <v>45969</v>
       </c>
       <c r="J47" s="22">
         <f>I47+G47</f>
@@ -3555,7 +3555,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="22" t="n">
-        <v>46031.26537644676</v>
+        <v>45960</v>
       </c>
       <c r="J5" s="22">
         <f>I5+G5</f>
@@ -3602,7 +3602,7 @@
         <v>3</v>
       </c>
       <c r="I6" s="22" t="n">
-        <v>46031.2653778383</v>
+        <v>45960</v>
       </c>
       <c r="J6" s="22">
         <f>I6+G6</f>
@@ -15540,7 +15540,7 @@
         <v>3</v>
       </c>
       <c r="I260" s="25" t="n">
-        <v>46031.26470364584</v>
+        <v>45983</v>
       </c>
       <c r="J260" s="22">
         <f>I260+G260</f>
@@ -16339,7 +16339,7 @@
         <v>3</v>
       </c>
       <c r="I277" s="22" t="n">
-        <v>46031.26355944444</v>
+        <v>45922</v>
       </c>
       <c r="J277" s="22">
         <f>I277+G277</f>

</xml_diff>